<commit_message>
final work of 4th sep csci 572
</commit_message>
<xml_diff>
--- a/homeworks_projects_CSCI572/hw1.xlsx
+++ b/homeworks_projects_CSCI572/hw1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="147">
   <si>
     <t>query 1</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -249,13 +249,264 @@
   </si>
   <si>
     <t>https://www.facebook.com/GouldLawLibrary</t>
+  </si>
+  <si>
+    <t>query 7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>google results</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>relevance score</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bing results</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>relevance score</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://gould.usc.edu/about/visit/</t>
+  </si>
+  <si>
+    <t>http://web-app.usc.edu/maps/</t>
+  </si>
+  <si>
+    <t>https://web-app.usc.edu/mobile/maps/?b=LAW</t>
+  </si>
+  <si>
+    <t>https://commencement.usc.edu/academic-school-ceremonies/gould/</t>
+  </si>
+  <si>
+    <t>Gould USC Map</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://gould.usc.edu/</t>
+  </si>
+  <si>
+    <t>http://www.bing.com/images/search?q=gould+usc+map&amp;qpvt=Gould+USC+Map</t>
+  </si>
+  <si>
+    <t>https://visit.usc.edu/maps-directions/</t>
+  </si>
+  <si>
+    <t>https://www.mapquest.com/us/california/schools-los-angeles/usc-gould-school-of-law-273286374</t>
+  </si>
+  <si>
+    <t>query 8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>google results</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>relevance score</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bing results</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/James_Brown_Scott</t>
+  </si>
+  <si>
+    <t>https://books.google.com/books?id=m1NKYCoJ1zgC&amp;pg=PA284&amp;lpg=PA284&amp;dq=James+Brown+ScoTT+Gould&amp;source=bl&amp;ots=pMGzvHferS&amp;sig=3OI-YjqJJOU_w4YhhVWM1wT-qZM&amp;hl=en&amp;sa=X&amp;ved=0ahUKEwik_Yfxn43WAhXHzFQKHVJZDqgQ6AEILDAB#v=onepage&amp;q=James%20Brown%20ScoTT%20Gould&amp;f=false</t>
+  </si>
+  <si>
+    <t>http://gould.usc.edu/about/history/timeline/</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/scottgouldjr/</t>
+  </si>
+  <si>
+    <t>https://books.google.com/books?id=76AiTZ-XQLUC&amp;pg=PA71&amp;lpg=PA71&amp;dq=James+Brown+ScoTT+Gould&amp;source=bl&amp;ots=G5jBLH4UIR&amp;sig=EOkFidIYrhlOAmqqhgJ8WIkCAzU&amp;hl=en&amp;sa=X&amp;ved=0ahUKEwik_Yfxn43WAhXHzFQKHVJZDqgQ6AEIQTAE#v=onepage&amp;q=James%20Brown%20ScoTT%20Gould&amp;f=false</t>
+  </si>
+  <si>
+    <t>James Brown Scott Gould</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/scott-gould-762378b2/</t>
+  </si>
+  <si>
+    <t>https://www.publishersmarketplace.com/members/rlrassociates/</t>
+  </si>
+  <si>
+    <t>http://www.metnews.com/articles/2009/reminiscing021209.htm</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/scottjamesgould/</t>
+  </si>
+  <si>
+    <t>https://www.intelius.com/people/Scott-Gould/Kalamazoo-MI/06SSADQF8WC</t>
+  </si>
+  <si>
+    <t>query 9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>USC GOULD Alumni</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>google results</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>relevance score</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bing results</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://gould.usc.edu/alumni/</t>
+  </si>
+  <si>
+    <t>http://gould.usc.edu/alumni/association/</t>
+  </si>
+  <si>
+    <t>http://gould.usc.edu/alumni/events/reunion/</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/USC-Gould-School-of-Law-Alumni-official-37479498635/</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/USC_Gould_School_of_Law</t>
+  </si>
+  <si>
+    <t>https://www.calsouthern.edu/info-law-by</t>
+  </si>
+  <si>
+    <t>http://gould.usc.edu/index.cfm</t>
+  </si>
+  <si>
+    <t>https://www.bing.com/maps?&amp;ty=18&amp;q=USC%20Gould%20School%20of%20Law%20Los%20Angeles%20CA&amp;ss=ypid.YN873x109496465&amp;ppois=34.0184593200684_-118.28450012207_USC%20Gould%20School%20of%20Law_YN873x109496465~&amp;cp=34.018459~-118.2845&amp;v=2&amp;sV=1</t>
+  </si>
+  <si>
+    <t>query 10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>USC law Undergraduate degree requirement</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>google result</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://degrees.jfku.edu/Law-Degrees_Landing-Page?&amp;utm_source=google&amp;utm_medium=ppc&amp;utm_term=%2Blaw%20%2Bdegrees&amp;mkwid=sd8PqKJEO|pcrid|214085611142|pkw|%2Blaw%20%2Bdegrees|pmt|b|pdv|c&amp;cvosrc=ppc.google.%2Blaw%20%2Bdegrees&amp;utm_campaign=Q317_Education_for_Change&amp;utm_adgroup=Law+Degree+-+BMM&amp;st-t=google&amp;vt-k=%2Blaw%20%2Bdegrees&amp;vt-mt=b&amp;source=</t>
+  </si>
+  <si>
+    <t>https://pages.northeastern.edu/UGUndergradSector2016-03InSegmentPaidSearch_LPFA.html?utm_campaign=mofu-sector&amp;utm_medium=search&amp;utm_source=google&amp;utm_content=c&amp;campaign=Undergraduate_Sector&amp;adgroup=General&amp;keyword=undergraduate%20degree&amp;gclid=EAIaIQobChMIutv-kamN1gIVDkR-Ch0HZQBOEAAYAiAAEgJ1EPD_BwE</t>
+  </si>
+  <si>
+    <t>http://gould.usc.edu/academics/degrees/jd/paths/3plus3/</t>
+  </si>
+  <si>
+    <t>http://gould.usc.edu/academics/degrees/jd/curriculum/requirements/</t>
+  </si>
+  <si>
+    <t>http://degrees.jfku.edu/Law-Degrees_Landing-Page?mkwid=78Hr81VN|pcrid|77378155920958|pkw|%2Blaw%20%2Bdegree|pmt|bb|pdv|c&amp;utm_source=bing&amp;utm_medium=ppc&amp;utm_term=%2Blaw%20%2Bdegree&amp;utm_campaign=JFKU_Law_California&amp;utm_adgroup=Law+Degree+-+HV+-+BMM&amp;cvosrc=ppc.bing.%2Blaw%20%2Bdegree&amp;st-t=bing&amp;vt-k=%2Blaw%20%2Bdegree&amp;vt-mt=bb&amp;source=</t>
+  </si>
+  <si>
+    <t>https://law.asu.edu/degree-programs/mls/mls-online/hr-concentration-mls?utm_source=bing&amp;utm_medium=cpc&amp;utm_term=MFDigi&amp;utm_source=bing&amp;utm_medium=cpc&amp;utm_campaign=Online%20-%20HR&amp;utm_term=employment%20law%20degree&amp;utm_content=HR%20Law%20Online</t>
+  </si>
+  <si>
+    <t>http://law.concordlawschool.edu/home/?adpos={adposition}&amp;creative={creative}&amp;device=c&amp;matchtype=b&amp;network=o&amp;source=SF08904&amp;ve=61599&amp;utm_source=MSN&amp;utm_medium=CPC&amp;utm_campaign=cls_lg_mer_NB_CA_GEO_GEN_MBR&amp;utm_term=86225217-VQ2-o-VQ6-{creative}-VQ16-c&amp;adid=3062834633</t>
+  </si>
+  <si>
+    <t>http://learn-more.umuc.edu/search/degree-programs/?marketcode=WB200880&amp;gclid=CIm2guiqjdYCFZIVfwod_6gOzg&amp;gclsrc=ds</t>
+  </si>
+  <si>
+    <t>http://catalogue.usc.edu/content.php?catoid=2&amp;navoid=263</t>
+  </si>
+  <si>
+    <t>query 11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>USC law master degree requirement</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://requestinfo.onlinelaw.pepperdine.edu/index1-d.html?experimentid=8561520362&amp;x=OFM&amp;s=search_nonbrand_google&amp;l=GGL%7CPEP-MLS%7CSEM%7CNBD%7CTIER1%7CBROAD%7CLegal%7COffline-Masters&amp;ef_id=c:198217243856_d:c_n:g_ti:kwd-301079764259&amp;gclid=EAIaIQobChMI0IrPrKuN1gIVQ19-Ch3NMgJhEAAYASAAEgK8kfD_BwE&amp;gclsrc=aw.ds</t>
+  </si>
+  <si>
+    <t>https://www.calsouthern.edu/info-llm-gaw?gclid=EAIaIQobChMI0IrPrKuN1gIVQ19-Ch3NMgJhEAAYAiAAEgKZmvD_BwE</t>
+  </si>
+  <si>
+    <t>http://degrees.jfku.edu/Law-Degrees_Landing-Page?&amp;utm_source=google&amp;utm_medium=ppc&amp;utm_term=%2Bmasters%20%2Blaw&amp;mkwid=sEmFV15La|pcrid|214071986529|pkw|%2Bmasters%20%2Blaw|pmt|b|pdv|c&amp;cvosrc=ppc.google.%2Bmasters%20%2Blaw&amp;utm_campaign=Q317_Education_for_Change&amp;utm_adgroup=Law+Masters+-+BMM&amp;st-t=google&amp;vt-k=%2Bmasters%20%2Blaw&amp;vt-mt=b&amp;source=</t>
+  </si>
+  <si>
+    <t>http://www.law.ac.uk/usa-ga/?utm_source=Adwords&amp;utm_medium=ppc&amp;utm_campaign=GUSIntPG&amp;utm_ID=10726&amp;mpch=ads</t>
+  </si>
+  <si>
+    <t>http://gould.usc.edu/academics/degrees/llm/</t>
+  </si>
+  <si>
+    <t>https://requestinfo.msw.usc.edu/index26.html?x=OFB&amp;s=search_brand_ybn&amp;l=YBN%7CUSC-MSW%7CSEM%7CBRD%7CTIER0%7CBROAD%7CBrand%7COffline&amp;ef_id=c:13836780198_d:c_n:o_ti:kwd-25627684967&amp;utm_source=bing&amp;utm_medium=cpc&amp;utm_campaign=YBN%7CUSC-MSW%7CSEM%7CBRD%7CTIER0%7CBROAD%7CBrand%7COffline&amp;utm_term=%2Busc%20%2Bdegree&amp;utm_content=YBN%7CUSC-MSW%7CSEM%7CBRD%7CTIER0%7CBROAD%7CBrand%7COffline%7CUSC%7CNon-Masters%7CDegree&amp;gclid=CMDNlNysjdYCFbccfgodRL4Jww&amp;gclsrc=ds&amp;experimentid=5380304957</t>
+  </si>
+  <si>
+    <t>https://requestinfo.msw.usc.edu/index26.html?x=OFB&amp;s=search_brand_ybn&amp;l=YBN%7CUSC-MSW%7CSEM%7CBRD%7CTIER0%7CBROAD%7CBrand%7COffline&amp;ef_id=c:13836780198_d:c_n:o_ti:kwd-25627684967&amp;utm_source=bing&amp;utm_medium=cpc&amp;utm_campaign=YBN%7CUSC-MSW%7CSEM%7CBRD%7CTIER0%7CBROAD%7CBrand%7COffline&amp;utm_term=%2Busc%20%2Bdegree&amp;utm_content=YBN%7CUSC-MSW%7CSEM%7CBRD%7CTIER0%7CBROAD%7CBrand%7COffline%7CUSC%7CNon-Masters%7CDegree&amp;gclid=COHukOusjdYCFRHYfgodkkUNhw&amp;gclsrc=ds&amp;experimentid=5380304957</t>
+  </si>
+  <si>
+    <t>http://uaonline.arizona.edu/law-ba?utm_source=bing&amp;utm_medium=cpc&amp;utm_campaign=BA_Law_PS&amp;utm_term=%2Blaw%20%2Bdegrees&amp;mm_campaign=554419A288EC44941164E483B26FC460&amp;KTCterm={keywordid}&amp;KTCGroup=1208363380743537&amp;KTCCampaign=276811051&amp;utm_content=LAW_law%20-%20degree</t>
+  </si>
+  <si>
+    <t>https://www.calsouthern.edu/info-llm-by</t>
+  </si>
+  <si>
+    <t>https://dornsife.usc.edu/masters-degrees/</t>
+  </si>
+  <si>
+    <t>query 12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://info.ncu.edu/onlinedegree2/?vt-dc&amp;vt-k=%2Bphd%20%2Bdegree&amp;adlvlkey&amp;adkey=DEFGGLGEN&amp;gclid=EAIaIQobChMI8uyEp62N1gIVWJN-Ch0z3ArhEAAYASAAEgJxYPD_BwE&amp;gclsrc=aw.ds</t>
+  </si>
+  <si>
+    <t>http://degrees.jfku.edu/Law-Degrees_Landing-Page?&amp;utm_source=google&amp;utm_medium=ppc&amp;utm_term=%2Blaw%20%2Bdegrees&amp;mkwid=sd8PqKJEO|pcrid|214085611145|pkw|%2Blaw%20%2Bdegrees|pmt|b|pdv|c&amp;cvosrc=ppc.google.%2Blaw%20%2Bdegrees&amp;utm_campaign=Q317_Education_for_Change&amp;utm_adgroup=Law+Degree+-+BMM&amp;st-t=google&amp;vt-k=%2Blaw%20%2Bdegrees&amp;vt-mt=b&amp;source=</t>
+  </si>
+  <si>
+    <t>http://learn.regent.edu/degree-programs/law/?bm_term=+law%20+degrees&amp;bm_matchtype=b&amp;bm_device=c&amp;bm_campaign=846142687&amp;bm_adgroup=40709905342&amp;bm_source=google&amp;bm_medium=ppc&amp;bm_target=kwd-306901681588&amp;bm_network=g&amp;gclid=EAIaIQobChMI8uyEp62N1gIVWJN-Ch0z3ArhEAAYAyAAEgJfIPD_BwE</t>
+  </si>
+  <si>
+    <t>https://pages.northeastern.edu/GCEDLPPSCH201603NationalSearch_LPFA.html?utm_medium=search&amp;utm_source=Google&amp;utm_campaign=mofu-niche&amp;utm_content=c&amp;campaign=Law_and_Policy_Doctorate&amp;adgroup=Law_and_Legal&amp;keyword=%252Blaw%2520%252Bphd&amp;gclid=EAIaIQobChMI8uyEp62N1gIVWJN-Ch0z3ArhEAAYBCAAEgLZEPD_BwE</t>
+  </si>
+  <si>
+    <t>http://gould.usc.edu/academics/degrees/jd/curriculum/dual-degrees/</t>
+  </si>
+  <si>
+    <t>usc law phd degree requirements</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://info.ncu.edu/onlinedegree2/?adlvlkey&amp;adkey=DEFBNG&amp;gclid=CICwkKqujdYCFRHYfgodkkUNhw&amp;gclsrc=ds</t>
+  </si>
+  <si>
+    <t>http://info.ncu.edu/onlinedegree2/?adlvlkey&amp;adkey=DEFBNG&amp;gclid=CIn46rKujdYCFUbpfgodabMOKg&amp;gclsrc=ds</t>
+  </si>
+  <si>
+    <t>https://law.asu.edu/degree-programs/mls/mls-online/intellectual-property-mls?utm_source=bing&amp;utm_medium=cpc&amp;utm_term=MFDigi&amp;utm_source=bing&amp;utm_medium=cpc&amp;utm_campaign=Online%20-%20IP&amp;utm_term=property%20law%20school&amp;utm_content=IP%20Law%20Online</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -280,6 +531,36 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -289,7 +570,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -297,6 +578,86 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -306,11 +667,107 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -615,655 +1072,1710 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H47"/>
+  <dimension ref="A1:J95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="H50" sqref="H50"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="E68" sqref="E68"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B2" t="s">
+    <row r="1" spans="1:9">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="4"/>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="5"/>
+      <c r="B2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C2" s="6"/>
+      <c r="D2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F2" t="s">
+      <c r="E2" s="6"/>
+      <c r="F2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="H2" t="s">
+      <c r="G2" s="6"/>
+      <c r="H2" s="6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1" t="s">
+      <c r="I2" s="7"/>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="5">
+        <v>1</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="C3" s="6"/>
+      <c r="D3" s="6">
+        <v>1</v>
+      </c>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="H3">
+      <c r="G3" s="6"/>
+      <c r="H3" s="6">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A4">
+      <c r="I3" s="7"/>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="5">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D4">
+      <c r="C4" s="6"/>
+      <c r="D4" s="6">
         <v>0.5</v>
       </c>
-      <c r="F4" t="s">
+      <c r="E4" s="6"/>
+      <c r="F4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A5">
+      <c r="G4" s="6"/>
+      <c r="H4" s="6">
+        <v>1</v>
+      </c>
+      <c r="I4" s="7"/>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="5">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D5">
+      <c r="C5" s="6"/>
+      <c r="D5" s="6">
         <v>0.25</v>
       </c>
-      <c r="F5" t="s">
+      <c r="E5" s="6"/>
+      <c r="F5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="H5">
+      <c r="G5" s="6"/>
+      <c r="H5" s="6">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A6">
+      <c r="I5" s="7"/>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="5">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D6">
+      <c r="C6" s="6"/>
+      <c r="D6" s="6">
         <v>0.25</v>
       </c>
-      <c r="F6" t="s">
+      <c r="E6" s="6"/>
+      <c r="F6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H6">
+      <c r="G6" s="6"/>
+      <c r="H6" s="6">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A7">
+      <c r="I6" s="7"/>
+    </row>
+    <row r="7" spans="1:9" ht="14.25" thickBot="1">
+      <c r="A7" s="9">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D7">
+      <c r="C7" s="10"/>
+      <c r="D7" s="10">
         <v>0.25</v>
       </c>
-      <c r="F7" t="s">
+      <c r="E7" s="10"/>
+      <c r="F7" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="H7">
+      <c r="G7" s="10"/>
+      <c r="H7" s="10">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A9" t="s">
+      <c r="I7" s="11"/>
+    </row>
+    <row r="8" spans="1:9" ht="14.25" thickBot="1"/>
+    <row r="9" spans="1:9">
+      <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B10" t="s">
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="4"/>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="5"/>
+      <c r="B10" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D10" t="s">
+      <c r="C10" s="6"/>
+      <c r="D10" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F10" t="s">
+      <c r="E10" s="6"/>
+      <c r="F10" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="H10" t="s">
+      <c r="G10" s="6"/>
+      <c r="H10" s="6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A11">
-        <v>1</v>
-      </c>
-      <c r="B11" t="s">
+      <c r="I10" s="7"/>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="5">
+        <v>1</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="F11" t="s">
+      <c r="C11" s="6"/>
+      <c r="D11" s="6">
+        <v>1</v>
+      </c>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="H11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A12">
+      <c r="G11" s="6"/>
+      <c r="H11" s="6">
+        <v>1</v>
+      </c>
+      <c r="I11" s="7"/>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="5">
         <v>2</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D12">
+      <c r="C12" s="6"/>
+      <c r="D12" s="6">
         <v>0.25</v>
       </c>
-      <c r="F12" t="s">
+      <c r="E12" s="6"/>
+      <c r="F12" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="H12">
+      <c r="G12" s="6"/>
+      <c r="H12" s="6">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A13">
+      <c r="I12" s="7"/>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="5">
         <v>3</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D13">
+      <c r="C13" s="6"/>
+      <c r="D13" s="6">
         <v>0.25</v>
       </c>
-      <c r="F13" t="s">
+      <c r="E13" s="6"/>
+      <c r="F13" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="H13">
+      <c r="G13" s="6"/>
+      <c r="H13" s="6">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A14">
+      <c r="I13" s="7"/>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="5">
         <v>4</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D14">
+      <c r="C14" s="6"/>
+      <c r="D14" s="6">
         <v>0.25</v>
       </c>
-      <c r="F14" t="s">
+      <c r="E14" s="6"/>
+      <c r="F14" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="H14">
+      <c r="G14" s="6"/>
+      <c r="H14" s="6">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A15">
+      <c r="I14" s="7"/>
+    </row>
+    <row r="15" spans="1:9" ht="14.25" thickBot="1">
+      <c r="A15" s="9">
         <v>5</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="D15">
+      <c r="C15" s="10"/>
+      <c r="D15" s="10">
         <v>0.25</v>
       </c>
-      <c r="F15" t="s">
+      <c r="E15" s="10"/>
+      <c r="F15" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="H15">
+      <c r="G15" s="10"/>
+      <c r="H15" s="10">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A17" t="s">
+      <c r="I15" s="11"/>
+    </row>
+    <row r="16" spans="1:9" ht="14.25" thickBot="1"/>
+    <row r="17" spans="1:9">
+      <c r="A17" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B18" t="s">
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="4"/>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="5"/>
+      <c r="B18" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D18" t="s">
+      <c r="C18" s="6"/>
+      <c r="D18" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F18" t="s">
+      <c r="E18" s="6"/>
+      <c r="F18" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="H18" t="s">
+      <c r="G18" s="6"/>
+      <c r="H18" s="6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A19">
-        <v>1</v>
-      </c>
-      <c r="B19" t="s">
+      <c r="I18" s="7"/>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="5">
+        <v>1</v>
+      </c>
+      <c r="B19" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D19">
+      <c r="C19" s="6"/>
+      <c r="D19" s="6">
         <v>0.25</v>
       </c>
-      <c r="F19" t="s">
+      <c r="E19" s="6"/>
+      <c r="F19" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="H19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A20">
+      <c r="G19" s="6"/>
+      <c r="H19" s="6">
+        <v>1</v>
+      </c>
+      <c r="I19" s="7"/>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" s="5">
         <v>2</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-      <c r="F20" t="s">
+      <c r="C20" s="6"/>
+      <c r="D20" s="6">
+        <v>1</v>
+      </c>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="H20">
+      <c r="G20" s="6"/>
+      <c r="H20" s="6">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A21">
+      <c r="I20" s="7"/>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" s="5">
         <v>3</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D21">
+      <c r="C21" s="6"/>
+      <c r="D21" s="6">
         <v>0.25</v>
       </c>
-      <c r="F21" t="s">
+      <c r="E21" s="6"/>
+      <c r="F21" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A22">
+      <c r="G21" s="6"/>
+      <c r="H21" s="6">
+        <v>0</v>
+      </c>
+      <c r="I21" s="7"/>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" s="5">
         <v>4</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
-      <c r="F22" t="s">
+      <c r="C22" s="6"/>
+      <c r="D22" s="6">
+        <v>0</v>
+      </c>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="H22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A23">
+      <c r="G22" s="6"/>
+      <c r="H22" s="6">
+        <v>0</v>
+      </c>
+      <c r="I22" s="7"/>
+    </row>
+    <row r="23" spans="1:9" ht="14.25" thickBot="1">
+      <c r="A23" s="9">
         <v>5</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D23">
-        <v>0</v>
-      </c>
-      <c r="F23" t="s">
+      <c r="C23" s="10"/>
+      <c r="D23" s="10">
+        <v>0</v>
+      </c>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="H23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A25" t="s">
+      <c r="G23" s="10"/>
+      <c r="H23" s="10">
+        <v>0</v>
+      </c>
+      <c r="I23" s="11"/>
+    </row>
+    <row r="24" spans="1:9" ht="14.25" thickBot="1"/>
+    <row r="25" spans="1:9">
+      <c r="A25" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="3" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B26" t="s">
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="4"/>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" s="5"/>
+      <c r="B26" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D26" t="s">
+      <c r="C26" s="6"/>
+      <c r="D26" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F26" t="s">
+      <c r="E26" s="6"/>
+      <c r="F26" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="H26" t="s">
+      <c r="G26" s="6"/>
+      <c r="H26" s="6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A27">
-        <v>1</v>
-      </c>
-      <c r="B27" t="s">
+      <c r="I26" s="7"/>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27" s="5">
+        <v>1</v>
+      </c>
+      <c r="B27" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="D27">
+      <c r="C27" s="6"/>
+      <c r="D27" s="6">
         <v>0.5</v>
       </c>
-      <c r="F27" t="s">
+      <c r="E27" s="6"/>
+      <c r="F27" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="H27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A28">
+      <c r="G27" s="6"/>
+      <c r="H27" s="6">
+        <v>0</v>
+      </c>
+      <c r="I27" s="7"/>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28" s="5">
         <v>2</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="D28">
+      <c r="C28" s="6"/>
+      <c r="D28" s="6">
         <v>0.5</v>
       </c>
-      <c r="F28" t="s">
+      <c r="E28" s="6"/>
+      <c r="F28" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="H28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A29">
+      <c r="G28" s="6"/>
+      <c r="H28" s="6">
+        <v>0</v>
+      </c>
+      <c r="I28" s="7"/>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29" s="5">
         <v>3</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D29">
-        <v>1</v>
-      </c>
-      <c r="F29" t="s">
+      <c r="C29" s="6"/>
+      <c r="D29" s="6">
+        <v>1</v>
+      </c>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="H29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A30">
+      <c r="G29" s="6"/>
+      <c r="H29" s="6">
+        <v>0</v>
+      </c>
+      <c r="I29" s="7"/>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30" s="5">
         <v>4</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D30">
-        <v>0</v>
-      </c>
-      <c r="F30" t="s">
+      <c r="C30" s="6"/>
+      <c r="D30" s="6">
+        <v>0</v>
+      </c>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="H30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A31">
+      <c r="G30" s="6"/>
+      <c r="H30" s="6">
+        <v>0</v>
+      </c>
+      <c r="I30" s="7"/>
+    </row>
+    <row r="31" spans="1:9" ht="14.25" thickBot="1">
+      <c r="A31" s="9">
         <v>5</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="D31">
-        <v>0</v>
-      </c>
-      <c r="F31" t="s">
+      <c r="C31" s="10"/>
+      <c r="D31" s="10">
+        <v>0</v>
+      </c>
+      <c r="E31" s="10"/>
+      <c r="F31" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="H31">
+      <c r="G31" s="10"/>
+      <c r="H31" s="10">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A33" t="s">
+      <c r="I31" s="11"/>
+    </row>
+    <row r="32" spans="1:9" ht="14.25" thickBot="1"/>
+    <row r="33" spans="1:9">
+      <c r="A33" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="3" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B34" t="s">
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="4"/>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34" s="5"/>
+      <c r="B34" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D34" t="s">
+      <c r="C34" s="6"/>
+      <c r="D34" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F34" t="s">
+      <c r="E34" s="6"/>
+      <c r="F34" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="H34" t="s">
+      <c r="G34" s="6"/>
+      <c r="H34" s="6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A35">
-        <v>1</v>
-      </c>
-      <c r="B35" t="s">
+      <c r="I34" s="7"/>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35" s="5">
+        <v>1</v>
+      </c>
+      <c r="B35" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D35">
-        <v>0</v>
-      </c>
-      <c r="F35" t="s">
+      <c r="C35" s="6"/>
+      <c r="D35" s="6">
+        <v>0</v>
+      </c>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="H35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A36">
+      <c r="G35" s="6"/>
+      <c r="H35" s="6">
+        <v>0</v>
+      </c>
+      <c r="I35" s="7"/>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="A36" s="5">
         <v>2</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="D36">
-        <v>0</v>
-      </c>
-      <c r="F36" t="s">
+      <c r="C36" s="6"/>
+      <c r="D36" s="6">
+        <v>0</v>
+      </c>
+      <c r="E36" s="6"/>
+      <c r="F36" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="H36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A37">
+      <c r="G36" s="6"/>
+      <c r="H36" s="6">
+        <v>0</v>
+      </c>
+      <c r="I36" s="7"/>
+    </row>
+    <row r="37" spans="1:9">
+      <c r="A37" s="5">
         <v>3</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="D37">
-        <v>0</v>
-      </c>
-      <c r="F37" t="s">
+      <c r="C37" s="6"/>
+      <c r="D37" s="6">
+        <v>0</v>
+      </c>
+      <c r="E37" s="6"/>
+      <c r="F37" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="H37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A38">
+      <c r="G37" s="6"/>
+      <c r="H37" s="6">
+        <v>0</v>
+      </c>
+      <c r="I37" s="7"/>
+    </row>
+    <row r="38" spans="1:9">
+      <c r="A38" s="5">
         <v>4</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="D38">
-        <v>0</v>
-      </c>
-      <c r="F38" t="s">
+      <c r="C38" s="6"/>
+      <c r="D38" s="6">
+        <v>0</v>
+      </c>
+      <c r="E38" s="6"/>
+      <c r="F38" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="H38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A39">
+      <c r="G38" s="6"/>
+      <c r="H38" s="6">
+        <v>0</v>
+      </c>
+      <c r="I38" s="7"/>
+    </row>
+    <row r="39" spans="1:9" ht="14.25" thickBot="1">
+      <c r="A39" s="9">
         <v>5</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="D39">
-        <v>1</v>
-      </c>
-      <c r="F39" t="s">
+      <c r="C39" s="10"/>
+      <c r="D39" s="10">
+        <v>1</v>
+      </c>
+      <c r="E39" s="10"/>
+      <c r="F39" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="H39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A41" t="s">
+      <c r="G39" s="10"/>
+      <c r="H39" s="10">
+        <v>1</v>
+      </c>
+      <c r="I39" s="11"/>
+    </row>
+    <row r="40" spans="1:9" ht="14.25" thickBot="1"/>
+    <row r="41" spans="1:9">
+      <c r="A41" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="3" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B42" t="s">
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="3"/>
+      <c r="H41" s="3"/>
+      <c r="I41" s="4"/>
+    </row>
+    <row r="42" spans="1:9">
+      <c r="A42" s="5"/>
+      <c r="B42" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="D42" t="s">
+      <c r="C42" s="6"/>
+      <c r="D42" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="F42" t="s">
+      <c r="E42" s="6"/>
+      <c r="F42" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="H42" t="s">
+      <c r="G42" s="6"/>
+      <c r="H42" s="6" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A43">
-        <v>1</v>
-      </c>
-      <c r="B43" t="s">
+      <c r="I42" s="7"/>
+    </row>
+    <row r="43" spans="1:9">
+      <c r="A43" s="5">
+        <v>1</v>
+      </c>
+      <c r="B43" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="D43">
-        <v>1</v>
-      </c>
-      <c r="F43" t="s">
+      <c r="C43" s="6"/>
+      <c r="D43" s="6">
+        <v>1</v>
+      </c>
+      <c r="E43" s="6"/>
+      <c r="F43" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="H43">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A44">
+      <c r="G43" s="6"/>
+      <c r="H43" s="6">
+        <v>0</v>
+      </c>
+      <c r="I43" s="7"/>
+    </row>
+    <row r="44" spans="1:9">
+      <c r="A44" s="5">
         <v>2</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="D44">
+      <c r="C44" s="6"/>
+      <c r="D44" s="6">
         <v>0.5</v>
       </c>
-      <c r="F44" t="s">
+      <c r="E44" s="6"/>
+      <c r="F44" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="H44">
+      <c r="G44" s="6"/>
+      <c r="H44" s="6">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A45">
+      <c r="I44" s="7"/>
+    </row>
+    <row r="45" spans="1:9">
+      <c r="A45" s="5">
         <v>3</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="D45">
+      <c r="C45" s="6"/>
+      <c r="D45" s="6">
         <v>0.5</v>
       </c>
-      <c r="F45" t="s">
+      <c r="E45" s="6"/>
+      <c r="F45" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="H45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A46">
+      <c r="G45" s="6"/>
+      <c r="H45" s="6">
+        <v>0</v>
+      </c>
+      <c r="I45" s="7"/>
+    </row>
+    <row r="46" spans="1:9">
+      <c r="A46" s="5">
         <v>4</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="D46">
+      <c r="C46" s="6"/>
+      <c r="D46" s="6">
         <v>0.5</v>
       </c>
-      <c r="F46" t="s">
+      <c r="E46" s="6"/>
+      <c r="F46" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="H46">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A47">
+      <c r="G46" s="6"/>
+      <c r="H46" s="6">
+        <v>0</v>
+      </c>
+      <c r="I46" s="7"/>
+    </row>
+    <row r="47" spans="1:9" ht="14.25" thickBot="1">
+      <c r="A47" s="9">
         <v>5</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="D47">
+      <c r="C47" s="10"/>
+      <c r="D47" s="10">
         <v>0.5</v>
       </c>
-      <c r="F47" t="s">
+      <c r="E47" s="10"/>
+      <c r="F47" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="H47">
+      <c r="G47" s="10"/>
+      <c r="H47" s="10">
         <v>0.5</v>
       </c>
+      <c r="I47" s="11"/>
+    </row>
+    <row r="48" spans="1:9" ht="14.25" thickBot="1"/>
+    <row r="49" spans="1:9">
+      <c r="A49" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C49" s="3"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="3"/>
+      <c r="F49" s="3"/>
+      <c r="G49" s="3"/>
+      <c r="H49" s="3"/>
+      <c r="I49" s="4"/>
+    </row>
+    <row r="50" spans="1:9">
+      <c r="A50" s="5"/>
+      <c r="B50" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C50" s="6"/>
+      <c r="D50" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E50" s="6"/>
+      <c r="F50" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="G50" s="6"/>
+      <c r="H50" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="I50" s="7"/>
+    </row>
+    <row r="51" spans="1:9">
+      <c r="A51" s="5">
+        <v>1</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C51" s="6"/>
+      <c r="D51" s="6">
+        <v>1</v>
+      </c>
+      <c r="E51" s="6"/>
+      <c r="F51" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="G51" s="6"/>
+      <c r="H51" s="6">
+        <v>1</v>
+      </c>
+      <c r="I51" s="7"/>
+    </row>
+    <row r="52" spans="1:9">
+      <c r="A52" s="5">
+        <v>2</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C52" s="6"/>
+      <c r="D52" s="6">
+        <v>0</v>
+      </c>
+      <c r="E52" s="6"/>
+      <c r="F52" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="G52" s="6"/>
+      <c r="H52" s="6">
+        <v>0</v>
+      </c>
+      <c r="I52" s="7"/>
+    </row>
+    <row r="53" spans="1:9">
+      <c r="A53" s="5">
+        <v>3</v>
+      </c>
+      <c r="B53" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C53" s="6"/>
+      <c r="D53" s="6">
+        <v>1</v>
+      </c>
+      <c r="E53" s="6"/>
+      <c r="F53" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="G53" s="6"/>
+      <c r="H53" s="6">
+        <v>1</v>
+      </c>
+      <c r="I53" s="7"/>
+    </row>
+    <row r="54" spans="1:9">
+      <c r="A54" s="5">
+        <v>4</v>
+      </c>
+      <c r="B54" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C54" s="6"/>
+      <c r="D54" s="6">
+        <v>0</v>
+      </c>
+      <c r="E54" s="6"/>
+      <c r="F54" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="G54" s="6"/>
+      <c r="H54" s="6">
+        <v>0</v>
+      </c>
+      <c r="I54" s="7"/>
+    </row>
+    <row r="55" spans="1:9" ht="14.25" thickBot="1">
+      <c r="A55" s="9">
+        <v>5</v>
+      </c>
+      <c r="B55" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="C55" s="10"/>
+      <c r="D55" s="10">
+        <v>0</v>
+      </c>
+      <c r="E55" s="10"/>
+      <c r="F55" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="G55" s="10"/>
+      <c r="H55" s="10">
+        <v>1</v>
+      </c>
+      <c r="I55" s="11"/>
+    </row>
+    <row r="56" spans="1:9" ht="14.25" thickBot="1"/>
+    <row r="57" spans="1:9">
+      <c r="A57" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C57" s="3"/>
+      <c r="D57" s="3"/>
+      <c r="E57" s="3"/>
+      <c r="F57" s="3"/>
+      <c r="G57" s="3"/>
+      <c r="H57" s="3"/>
+      <c r="I57" s="4"/>
+    </row>
+    <row r="58" spans="1:9">
+      <c r="A58" s="5"/>
+      <c r="B58" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C58" s="6"/>
+      <c r="D58" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="E58" s="6"/>
+      <c r="F58" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="G58" s="6"/>
+      <c r="H58" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="I58" s="7"/>
+    </row>
+    <row r="59" spans="1:9">
+      <c r="A59" s="5">
+        <v>1</v>
+      </c>
+      <c r="B59" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="C59" s="6"/>
+      <c r="D59" s="6">
+        <v>1</v>
+      </c>
+      <c r="E59" s="6"/>
+      <c r="F59" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="G59" s="6"/>
+      <c r="H59" s="6">
+        <v>0</v>
+      </c>
+      <c r="I59" s="7"/>
+    </row>
+    <row r="60" spans="1:9">
+      <c r="A60" s="5">
+        <v>2</v>
+      </c>
+      <c r="B60" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C60" s="6"/>
+      <c r="D60" s="6">
+        <v>0</v>
+      </c>
+      <c r="E60" s="6"/>
+      <c r="F60" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="G60" s="6"/>
+      <c r="H60" s="6">
+        <v>0</v>
+      </c>
+      <c r="I60" s="7"/>
+    </row>
+    <row r="61" spans="1:9">
+      <c r="A61" s="5">
+        <v>3</v>
+      </c>
+      <c r="B61" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C61" s="6"/>
+      <c r="D61" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="E61" s="6"/>
+      <c r="F61" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="G61" s="6"/>
+      <c r="H61" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="I61" s="7"/>
+    </row>
+    <row r="62" spans="1:9">
+      <c r="A62" s="5">
+        <v>4</v>
+      </c>
+      <c r="B62" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C62" s="6"/>
+      <c r="D62" s="6">
+        <v>0</v>
+      </c>
+      <c r="E62" s="6"/>
+      <c r="F62" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="G62" s="6"/>
+      <c r="H62" s="6">
+        <v>0</v>
+      </c>
+      <c r="I62" s="7"/>
+    </row>
+    <row r="63" spans="1:9" ht="14.25" thickBot="1">
+      <c r="A63" s="9">
+        <v>5</v>
+      </c>
+      <c r="B63" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="C63" s="10"/>
+      <c r="D63" s="10">
+        <v>0</v>
+      </c>
+      <c r="E63" s="10"/>
+      <c r="F63" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="G63" s="10"/>
+      <c r="H63" s="10">
+        <v>0</v>
+      </c>
+      <c r="I63" s="11"/>
+    </row>
+    <row r="64" spans="1:9" ht="14.25" thickBot="1"/>
+    <row r="65" spans="1:10">
+      <c r="A65" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="B65" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="C65" s="14"/>
+      <c r="D65" s="14"/>
+      <c r="E65" s="14"/>
+      <c r="F65" s="14"/>
+      <c r="G65" s="14"/>
+      <c r="H65" s="14"/>
+      <c r="I65" s="15"/>
+    </row>
+    <row r="66" spans="1:10">
+      <c r="A66" s="16"/>
+      <c r="B66" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="C66" s="17"/>
+      <c r="D66" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="E66" s="17"/>
+      <c r="F66" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="G66" s="17"/>
+      <c r="H66" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="I66" s="18"/>
+    </row>
+    <row r="67" spans="1:10">
+      <c r="A67" s="16">
+        <v>1</v>
+      </c>
+      <c r="B67" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="C67" s="17"/>
+      <c r="D67" s="17">
+        <v>1</v>
+      </c>
+      <c r="E67" s="17"/>
+      <c r="F67" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="G67" s="17"/>
+      <c r="H67" s="17">
+        <v>0.25</v>
+      </c>
+      <c r="I67" s="18"/>
+    </row>
+    <row r="68" spans="1:10">
+      <c r="A68" s="16">
+        <v>2</v>
+      </c>
+      <c r="B68" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="C68" s="17"/>
+      <c r="D68" s="17">
+        <v>1</v>
+      </c>
+      <c r="E68" s="17"/>
+      <c r="F68" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="G68" s="17"/>
+      <c r="H68" s="17">
+        <v>0</v>
+      </c>
+      <c r="I68" s="18"/>
+    </row>
+    <row r="69" spans="1:10">
+      <c r="A69" s="16">
+        <v>3</v>
+      </c>
+      <c r="B69" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="C69" s="17"/>
+      <c r="D69" s="17">
+        <v>1</v>
+      </c>
+      <c r="E69" s="17"/>
+      <c r="F69" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="G69" s="17"/>
+      <c r="H69" s="17">
+        <v>0</v>
+      </c>
+      <c r="I69" s="18"/>
+    </row>
+    <row r="70" spans="1:10">
+      <c r="A70" s="16">
+        <v>4</v>
+      </c>
+      <c r="B70" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="C70" s="17"/>
+      <c r="D70" s="17">
+        <v>1</v>
+      </c>
+      <c r="E70" s="17"/>
+      <c r="F70" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="G70" s="17"/>
+      <c r="H70" s="17">
+        <v>0</v>
+      </c>
+      <c r="I70" s="18"/>
+    </row>
+    <row r="71" spans="1:10" ht="14.25" thickBot="1">
+      <c r="A71" s="19">
+        <v>5</v>
+      </c>
+      <c r="B71" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="C71" s="20"/>
+      <c r="D71" s="20">
+        <v>0</v>
+      </c>
+      <c r="E71" s="20"/>
+      <c r="F71" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="G71" s="20"/>
+      <c r="H71" s="20">
+        <v>0</v>
+      </c>
+      <c r="I71" s="21"/>
+    </row>
+    <row r="72" spans="1:10" ht="14.25" thickBot="1"/>
+    <row r="73" spans="1:10">
+      <c r="A73" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="B73" s="23" t="s">
+        <v>114</v>
+      </c>
+      <c r="C73" s="24"/>
+      <c r="D73" s="24"/>
+      <c r="E73" s="24"/>
+      <c r="F73" s="24"/>
+      <c r="G73" s="24"/>
+      <c r="H73" s="24"/>
+      <c r="I73" s="25"/>
+      <c r="J73" s="1"/>
+    </row>
+    <row r="74" spans="1:10">
+      <c r="A74" s="26"/>
+      <c r="B74" s="27" t="s">
+        <v>115</v>
+      </c>
+      <c r="C74" s="28"/>
+      <c r="D74" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="E74" s="28"/>
+      <c r="F74" s="27" t="s">
+        <v>104</v>
+      </c>
+      <c r="G74" s="28"/>
+      <c r="H74" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="I74" s="29"/>
+      <c r="J74" s="1"/>
+    </row>
+    <row r="75" spans="1:10">
+      <c r="A75" s="26">
+        <v>1</v>
+      </c>
+      <c r="B75" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="C75" s="28"/>
+      <c r="D75" s="28">
+        <v>0</v>
+      </c>
+      <c r="E75" s="28"/>
+      <c r="F75" s="30" t="s">
+        <v>120</v>
+      </c>
+      <c r="G75" s="28"/>
+      <c r="H75" s="28">
+        <v>0</v>
+      </c>
+      <c r="I75" s="29"/>
+      <c r="J75" s="1"/>
+    </row>
+    <row r="76" spans="1:10">
+      <c r="A76" s="26">
+        <v>2</v>
+      </c>
+      <c r="B76" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="C76" s="28"/>
+      <c r="D76" s="28">
+        <v>0</v>
+      </c>
+      <c r="E76" s="28"/>
+      <c r="F76" s="28" t="s">
+        <v>121</v>
+      </c>
+      <c r="G76" s="28"/>
+      <c r="H76" s="28">
+        <v>0</v>
+      </c>
+      <c r="I76" s="29"/>
+      <c r="J76" s="1"/>
+    </row>
+    <row r="77" spans="1:10">
+      <c r="A77" s="26">
+        <v>3</v>
+      </c>
+      <c r="B77" s="28" t="s">
+        <v>118</v>
+      </c>
+      <c r="C77" s="28"/>
+      <c r="D77" s="28">
+        <v>0</v>
+      </c>
+      <c r="E77" s="28"/>
+      <c r="F77" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="G77" s="28"/>
+      <c r="H77" s="28">
+        <v>0</v>
+      </c>
+      <c r="I77" s="29"/>
+      <c r="J77" s="1"/>
+    </row>
+    <row r="78" spans="1:10">
+      <c r="A78" s="26">
+        <v>4</v>
+      </c>
+      <c r="B78" s="28" t="s">
+        <v>119</v>
+      </c>
+      <c r="C78" s="28"/>
+      <c r="D78" s="28">
+        <v>1</v>
+      </c>
+      <c r="E78" s="28"/>
+      <c r="F78" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="G78" s="28"/>
+      <c r="H78" s="28">
+        <v>0</v>
+      </c>
+      <c r="I78" s="29"/>
+      <c r="J78" s="1"/>
+    </row>
+    <row r="79" spans="1:10" ht="14.25" thickBot="1">
+      <c r="A79" s="31">
+        <v>5</v>
+      </c>
+      <c r="B79" s="32" t="s">
+        <v>118</v>
+      </c>
+      <c r="C79" s="32"/>
+      <c r="D79" s="32">
+        <v>0</v>
+      </c>
+      <c r="E79" s="32"/>
+      <c r="F79" s="32" t="s">
+        <v>124</v>
+      </c>
+      <c r="G79" s="32"/>
+      <c r="H79" s="32">
+        <v>1</v>
+      </c>
+      <c r="I79" s="33"/>
+      <c r="J79" s="1"/>
+    </row>
+    <row r="80" spans="1:10" ht="14.25" thickBot="1">
+      <c r="A80" s="1"/>
+      <c r="B80" s="1"/>
+      <c r="C80" s="1"/>
+      <c r="D80" s="1"/>
+      <c r="E80" s="1"/>
+      <c r="F80" s="1"/>
+      <c r="G80" s="1"/>
+      <c r="H80" s="1"/>
+      <c r="I80" s="1"/>
+      <c r="J80" s="1"/>
+    </row>
+    <row r="81" spans="1:9">
+      <c r="A81" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B81" s="24" t="s">
+        <v>126</v>
+      </c>
+      <c r="C81" s="3"/>
+      <c r="D81" s="3"/>
+      <c r="E81" s="3"/>
+      <c r="F81" s="3"/>
+      <c r="G81" s="3"/>
+      <c r="H81" s="3"/>
+      <c r="I81" s="4"/>
+    </row>
+    <row r="82" spans="1:9">
+      <c r="A82" s="5"/>
+      <c r="B82" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="C82" s="6"/>
+      <c r="D82" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="E82" s="6"/>
+      <c r="F82" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="G82" s="6"/>
+      <c r="H82" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="I82" s="7"/>
+    </row>
+    <row r="83" spans="1:9">
+      <c r="A83" s="5">
+        <v>1</v>
+      </c>
+      <c r="B83" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="C83" s="6"/>
+      <c r="D83" s="6">
+        <v>0</v>
+      </c>
+      <c r="E83" s="6"/>
+      <c r="F83" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="G83" s="6"/>
+      <c r="H83" s="6">
+        <v>0</v>
+      </c>
+      <c r="I83" s="7"/>
+    </row>
+    <row r="84" spans="1:9">
+      <c r="A84" s="5">
+        <v>2</v>
+      </c>
+      <c r="B84" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="C84" s="6"/>
+      <c r="D84" s="6">
+        <v>0</v>
+      </c>
+      <c r="E84" s="6"/>
+      <c r="F84" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="G84" s="6"/>
+      <c r="H84" s="6">
+        <v>0</v>
+      </c>
+      <c r="I84" s="7"/>
+    </row>
+    <row r="85" spans="1:9">
+      <c r="A85" s="5">
+        <v>3</v>
+      </c>
+      <c r="B85" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="C85" s="6"/>
+      <c r="D85" s="6">
+        <v>0</v>
+      </c>
+      <c r="E85" s="6"/>
+      <c r="F85" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="G85" s="6"/>
+      <c r="H85" s="6">
+        <v>0</v>
+      </c>
+      <c r="I85" s="7"/>
+    </row>
+    <row r="86" spans="1:9">
+      <c r="A86" s="5">
+        <v>4</v>
+      </c>
+      <c r="B86" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="C86" s="6"/>
+      <c r="D86" s="6">
+        <v>0</v>
+      </c>
+      <c r="E86" s="6"/>
+      <c r="F86" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="G86" s="6"/>
+      <c r="H86" s="6">
+        <v>0</v>
+      </c>
+      <c r="I86" s="7"/>
+    </row>
+    <row r="87" spans="1:9" ht="14.25" thickBot="1">
+      <c r="A87" s="9">
+        <v>5</v>
+      </c>
+      <c r="B87" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="C87" s="10"/>
+      <c r="D87" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="E87" s="10"/>
+      <c r="F87" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="G87" s="10"/>
+      <c r="H87" s="10">
+        <v>0</v>
+      </c>
+      <c r="I87" s="11"/>
+    </row>
+    <row r="88" spans="1:9" ht="14.25" thickBot="1"/>
+    <row r="89" spans="1:9">
+      <c r="A89" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="C89" s="3"/>
+      <c r="D89" s="3"/>
+      <c r="E89" s="3"/>
+      <c r="F89" s="3"/>
+      <c r="G89" s="3"/>
+      <c r="H89" s="3"/>
+      <c r="I89" s="4"/>
+    </row>
+    <row r="90" spans="1:9">
+      <c r="A90" s="5"/>
+      <c r="B90" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="C90" s="6"/>
+      <c r="D90" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="E90" s="6"/>
+      <c r="F90" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="G90" s="6"/>
+      <c r="H90" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="I90" s="7"/>
+    </row>
+    <row r="91" spans="1:9">
+      <c r="A91" s="5">
+        <v>1</v>
+      </c>
+      <c r="B91" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="C91" s="6"/>
+      <c r="D91" s="6">
+        <v>0</v>
+      </c>
+      <c r="E91" s="6"/>
+      <c r="F91" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="G91" s="6"/>
+      <c r="H91" s="6">
+        <v>0</v>
+      </c>
+      <c r="I91" s="7"/>
+    </row>
+    <row r="92" spans="1:9">
+      <c r="A92" s="5">
+        <v>2</v>
+      </c>
+      <c r="B92" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="C92" s="6"/>
+      <c r="D92" s="6">
+        <v>0</v>
+      </c>
+      <c r="E92" s="6"/>
+      <c r="F92" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="G92" s="6"/>
+      <c r="H92" s="6">
+        <v>0</v>
+      </c>
+      <c r="I92" s="7"/>
+    </row>
+    <row r="93" spans="1:9">
+      <c r="A93" s="5">
+        <v>3</v>
+      </c>
+      <c r="B93" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="C93" s="6"/>
+      <c r="D93" s="6">
+        <v>0</v>
+      </c>
+      <c r="E93" s="6"/>
+      <c r="F93" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="G93" s="6"/>
+      <c r="H93" s="6">
+        <v>0</v>
+      </c>
+      <c r="I93" s="7"/>
+    </row>
+    <row r="94" spans="1:9">
+      <c r="A94" s="5">
+        <v>4</v>
+      </c>
+      <c r="B94" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="C94" s="6"/>
+      <c r="D94" s="6">
+        <v>0</v>
+      </c>
+      <c r="E94" s="6"/>
+      <c r="F94" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="G94" s="6"/>
+      <c r="H94" s="6">
+        <v>0</v>
+      </c>
+      <c r="I94" s="7"/>
+    </row>
+    <row r="95" spans="1:9" ht="14.25" thickBot="1">
+      <c r="A95" s="9">
+        <v>5</v>
+      </c>
+      <c r="B95" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="C95" s="10"/>
+      <c r="D95" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="E95" s="10"/>
+      <c r="F95" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="G95" s="10"/>
+      <c r="H95" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="I95" s="11"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1271,6 +2783,7 @@
     <hyperlink ref="B3" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1280,7 +2793,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1293,7 +2806,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fixed final result of hw1
</commit_message>
<xml_diff>
--- a/homeworks_projects_CSCI572/hw1.xlsx
+++ b/homeworks_projects_CSCI572/hw1.xlsx
@@ -486,10 +486,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>usc law phd degree requirements</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>http://gould.usc.edu/why/academics/cle/</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -610,10 +606,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>usc law phd degree requirements</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>http://catalogue.usc.edu/content.php?catoid=2&amp;navoid=303</t>
   </si>
   <si>
@@ -689,6 +681,13 @@
   <si>
     <t>query</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>usc law doctor degree requirements</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://gould.usc.edu/academics/degrees/jd/curriculum/overview/</t>
   </si>
 </sst>
 </file>
@@ -1024,11 +1023,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="22285312"/>
-        <c:axId val="195037440"/>
+        <c:axId val="192210944"/>
+        <c:axId val="189707328"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="22285312"/>
+        <c:axId val="192210944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1037,7 +1036,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="195037440"/>
+        <c:crossAx val="189707328"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1045,7 +1044,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="195037440"/>
+        <c:axId val="189707328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1058,7 +1057,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="22285312"/>
+        <c:crossAx val="192210944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1174,11 +1173,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="48614400"/>
-        <c:axId val="195039168"/>
+        <c:axId val="199282688"/>
+        <c:axId val="199193088"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="48614400"/>
+        <c:axId val="199282688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1187,7 +1186,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="195039168"/>
+        <c:crossAx val="199193088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1195,7 +1194,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="195039168"/>
+        <c:axId val="199193088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1208,7 +1207,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48614400"/>
+        <c:crossAx val="199282688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1324,11 +1323,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="191107072"/>
-        <c:axId val="282408000"/>
+        <c:axId val="199283200"/>
+        <c:axId val="199194816"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="191107072"/>
+        <c:axId val="199283200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1337,7 +1336,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="282408000"/>
+        <c:crossAx val="199194816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1345,7 +1344,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="282408000"/>
+        <c:axId val="199194816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1358,7 +1357,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="191107072"/>
+        <c:crossAx val="199283200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1474,11 +1473,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="144621568"/>
-        <c:axId val="285774336"/>
+        <c:axId val="199283712"/>
+        <c:axId val="199393280"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="144621568"/>
+        <c:axId val="199283712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1487,7 +1486,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="285774336"/>
+        <c:crossAx val="199393280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1495,7 +1494,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="285774336"/>
+        <c:axId val="199393280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1508,7 +1507,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="144621568"/>
+        <c:crossAx val="199283712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1624,11 +1623,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="191108608"/>
-        <c:axId val="217682432"/>
+        <c:axId val="199284224"/>
+        <c:axId val="199395008"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="191108608"/>
+        <c:axId val="199284224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1637,7 +1636,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="217682432"/>
+        <c:crossAx val="199395008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1645,7 +1644,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="217682432"/>
+        <c:axId val="199395008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1658,7 +1657,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="191108608"/>
+        <c:crossAx val="199284224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1770,11 +1769,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="195256832"/>
-        <c:axId val="282408576"/>
+        <c:axId val="199284736"/>
+        <c:axId val="199396736"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="195256832"/>
+        <c:axId val="199284736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1783,7 +1782,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="282408576"/>
+        <c:crossAx val="199396736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1791,7 +1790,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="282408576"/>
+        <c:axId val="199396736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5"/>
@@ -1804,7 +1803,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="195256832"/>
+        <c:crossAx val="199284736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1944,11 +1943,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="190973440"/>
-        <c:axId val="285776064"/>
+        <c:axId val="199285760"/>
+        <c:axId val="199398464"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="190973440"/>
+        <c:axId val="199285760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1957,7 +1956,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="285776064"/>
+        <c:crossAx val="199398464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1965,7 +1964,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="285776064"/>
+        <c:axId val="199398464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5"/>
@@ -1978,7 +1977,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="190973440"/>
+        <c:crossAx val="199285760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2118,11 +2117,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="179090944"/>
-        <c:axId val="216307904"/>
+        <c:axId val="199286272"/>
+        <c:axId val="199400192"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="179090944"/>
+        <c:axId val="199286272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2131,7 +2130,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="216307904"/>
+        <c:crossAx val="199400192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2139,7 +2138,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="216307904"/>
+        <c:axId val="199400192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5"/>
@@ -2152,7 +2151,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="179090944"/>
+        <c:crossAx val="199286272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2292,11 +2291,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="195256320"/>
-        <c:axId val="217678976"/>
+        <c:axId val="198947840"/>
+        <c:axId val="199836800"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="195256320"/>
+        <c:axId val="198947840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2306,7 +2305,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="217678976"/>
+        <c:crossAx val="199836800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2314,7 +2313,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="217678976"/>
+        <c:axId val="199836800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5"/>
@@ -2327,7 +2326,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="195256320"/>
+        <c:crossAx val="198947840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2467,11 +2466,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="195257344"/>
-        <c:axId val="283042944"/>
+        <c:axId val="199675904"/>
+        <c:axId val="199838528"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="195257344"/>
+        <c:axId val="199675904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2481,7 +2480,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="283042944"/>
+        <c:crossAx val="199838528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2489,7 +2488,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="283042944"/>
+        <c:axId val="199838528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5"/>
@@ -2502,7 +2501,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="195257344"/>
+        <c:crossAx val="199675904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2618,11 +2617,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="22617088"/>
-        <c:axId val="195042624"/>
+        <c:axId val="198946816"/>
+        <c:axId val="189709056"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="22617088"/>
+        <c:axId val="198946816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2631,7 +2630,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="195042624"/>
+        <c:crossAx val="189709056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2639,7 +2638,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="195042624"/>
+        <c:axId val="189709056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2652,7 +2651,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="22617088"/>
+        <c:crossAx val="198946816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2768,11 +2767,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="144622592"/>
-        <c:axId val="281832256"/>
+        <c:axId val="198947328"/>
+        <c:axId val="197943872"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="144622592"/>
+        <c:axId val="198947328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2781,7 +2780,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="281832256"/>
+        <c:crossAx val="197943872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2789,7 +2788,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="281832256"/>
+        <c:axId val="197943872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2802,7 +2801,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="144622592"/>
+        <c:crossAx val="198947328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2918,11 +2917,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="144624128"/>
-        <c:axId val="281835712"/>
+        <c:axId val="198948352"/>
+        <c:axId val="197945600"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="144624128"/>
+        <c:axId val="198948352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2931,7 +2930,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="281835712"/>
+        <c:crossAx val="197945600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2939,7 +2938,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="281835712"/>
+        <c:axId val="197945600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2952,7 +2951,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="144624128"/>
+        <c:crossAx val="198948352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3068,11 +3067,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="190974976"/>
-        <c:axId val="238264320"/>
+        <c:axId val="198948864"/>
+        <c:axId val="197947328"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="190974976"/>
+        <c:axId val="198948864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3081,7 +3080,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="238264320"/>
+        <c:crossAx val="197947328"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3089,7 +3088,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="238264320"/>
+        <c:axId val="197947328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -3102,7 +3101,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="190974976"/>
+        <c:crossAx val="198948864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3218,11 +3217,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="144980992"/>
-        <c:axId val="238271232"/>
+        <c:axId val="198949376"/>
+        <c:axId val="197949056"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="144980992"/>
+        <c:axId val="198949376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3231,7 +3230,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="238271232"/>
+        <c:crossAx val="197949056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3239,7 +3238,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="238271232"/>
+        <c:axId val="197949056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -3252,7 +3251,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="144980992"/>
+        <c:crossAx val="198949376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3368,11 +3367,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="190064640"/>
-        <c:axId val="282403392"/>
+        <c:axId val="198949888"/>
+        <c:axId val="197950784"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="190064640"/>
+        <c:axId val="198949888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3381,7 +3380,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="282403392"/>
+        <c:crossAx val="197950784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3389,7 +3388,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="282403392"/>
+        <c:axId val="197950784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -3402,7 +3401,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="190064640"/>
+        <c:crossAx val="198949888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3518,11 +3517,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="190975488"/>
-        <c:axId val="282406848"/>
+        <c:axId val="198950400"/>
+        <c:axId val="199189632"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="190975488"/>
+        <c:axId val="198950400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3531,7 +3530,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="282406848"/>
+        <c:crossAx val="199189632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3539,7 +3538,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="282406848"/>
+        <c:axId val="199189632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -3552,7 +3551,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="190975488"/>
+        <c:crossAx val="198950400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3668,11 +3667,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="48613376"/>
-        <c:axId val="282410304"/>
+        <c:axId val="192209408"/>
+        <c:axId val="199191360"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="48613376"/>
+        <c:axId val="192209408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3681,7 +3680,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="282410304"/>
+        <c:crossAx val="199191360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3689,7 +3688,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="282410304"/>
+        <c:axId val="199191360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -3702,7 +3701,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48613376"/>
+        <c:crossAx val="192209408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4266,6 +4265,113 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>182</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>191</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3314700" y="31642050"/>
+          <a:ext cx="6734175" cy="1504950"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1600">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>conclusion: for question 1:which is better considering first 5 search:my answer is google  perform better than bing because for top 5 search, higher relevance score result always comes to top compare to bing</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="zh-CN" sz="1600">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1600">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>for question 2:for the navigational query and informational query:bing and google nearly have no different compare to each other</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="zh-CN" sz="1600">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4558,8 +4664,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T164"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
-      <selection activeCell="H243" sqref="H243"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P188" sqref="P188"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -5190,7 +5296,7 @@
         <v>1</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C35" s="6"/>
       <c r="D35" s="6">
@@ -5211,7 +5317,7 @@
         <v>2</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C36" s="6"/>
       <c r="D36" s="6">
@@ -5219,7 +5325,7 @@
       </c>
       <c r="E36" s="6"/>
       <c r="F36" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G36" s="6"/>
       <c r="H36" s="6">
@@ -5232,7 +5338,7 @@
         <v>3</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C37" s="6"/>
       <c r="D37" s="6">
@@ -5240,7 +5346,7 @@
       </c>
       <c r="E37" s="6"/>
       <c r="F37" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G37" s="6"/>
       <c r="H37" s="6">
@@ -5253,7 +5359,7 @@
         <v>4</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C38" s="6"/>
       <c r="D38" s="6">
@@ -5261,7 +5367,7 @@
       </c>
       <c r="E38" s="6"/>
       <c r="F38" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G38" s="6"/>
       <c r="H38" s="6">
@@ -5274,7 +5380,7 @@
         <v>5</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C39" s="9"/>
       <c r="D39" s="9">
@@ -5282,7 +5388,7 @@
       </c>
       <c r="E39" s="9"/>
       <c r="F39" s="9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G39" s="9"/>
       <c r="H39" s="9">
@@ -5623,7 +5729,7 @@
         <v>118</v>
       </c>
       <c r="S58" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="T58" t="s">
         <v>107</v>
@@ -5924,7 +6030,7 @@
       </c>
       <c r="E75" s="17"/>
       <c r="F75" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G75" s="17"/>
       <c r="H75" s="17">
@@ -5938,7 +6044,7 @@
         <v>2</v>
       </c>
       <c r="B76" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C76" s="17"/>
       <c r="D76" s="17">
@@ -5960,7 +6066,7 @@
         <v>3</v>
       </c>
       <c r="B77" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C77" s="17"/>
       <c r="D77" s="17">
@@ -5968,7 +6074,7 @@
       </c>
       <c r="E77" s="17"/>
       <c r="F77" s="17" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G77" s="17"/>
       <c r="H77" s="17">
@@ -6002,7 +6108,7 @@
       </c>
       <c r="E78" s="17"/>
       <c r="F78" s="17" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G78" s="17"/>
       <c r="H78" s="17">
@@ -6024,7 +6130,7 @@
       </c>
       <c r="E79" s="20"/>
       <c r="F79" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G79" s="20"/>
       <c r="H79" s="20">
@@ -6105,7 +6211,7 @@
         <v>2</v>
       </c>
       <c r="B84" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C84" s="6"/>
       <c r="D84" s="6">
@@ -6134,7 +6240,7 @@
       </c>
       <c r="E85" s="6"/>
       <c r="F85" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G85" s="6"/>
       <c r="H85" s="6">
@@ -6147,7 +6253,7 @@
         <v>4</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C86" s="6"/>
       <c r="D86" s="22">
@@ -6155,7 +6261,7 @@
       </c>
       <c r="E86" s="6"/>
       <c r="F86" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G86" s="6"/>
       <c r="H86" s="22">
@@ -6168,7 +6274,7 @@
         <v>5</v>
       </c>
       <c r="B87" s="9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C87" s="9"/>
       <c r="D87" s="9">
@@ -6176,7 +6282,7 @@
       </c>
       <c r="E87" s="9"/>
       <c r="F87" s="9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G87" s="9"/>
       <c r="H87" s="9">
@@ -6190,7 +6296,7 @@
         <v>105</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>175</v>
+        <v>194</v>
       </c>
       <c r="C89" s="3"/>
       <c r="D89" s="3"/>
@@ -6224,7 +6330,7 @@
         <v>1</v>
       </c>
       <c r="B91" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C91" s="6"/>
       <c r="D91" s="6">
@@ -6245,7 +6351,7 @@
         <v>2</v>
       </c>
       <c r="B92" s="6" t="s">
-        <v>100</v>
+        <v>195</v>
       </c>
       <c r="C92" s="6"/>
       <c r="D92" s="6">
@@ -6287,7 +6393,7 @@
         <v>4</v>
       </c>
       <c r="B94" s="6" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C94" s="6"/>
       <c r="D94" s="22">
@@ -6308,7 +6414,7 @@
         <v>5</v>
       </c>
       <c r="B95" s="9" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C95" s="9"/>
       <c r="D95" s="9">
@@ -6316,7 +6422,7 @@
       </c>
       <c r="E95" s="9"/>
       <c r="F95" s="9" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="G95" s="9"/>
       <c r="H95" s="9">
@@ -6335,16 +6441,16 @@
         <v>137</v>
       </c>
       <c r="T96" t="s">
-        <v>138</v>
+        <v>194</v>
       </c>
     </row>
     <row r="97" spans="1:9" ht="14.25" thickBot="1"/>
     <row r="98" spans="1:9">
       <c r="A98" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B98" s="3" t="s">
         <v>160</v>
-      </c>
-      <c r="B98" s="3" t="s">
-        <v>161</v>
       </c>
       <c r="C98" s="3"/>
       <c r="D98" s="3"/>
@@ -6357,19 +6463,19 @@
     <row r="99" spans="1:9">
       <c r="A99" s="5"/>
       <c r="B99" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C99" s="6"/>
       <c r="D99" s="6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E99" s="6"/>
       <c r="F99" s="6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G99" s="6"/>
       <c r="H99" s="6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I99" s="7"/>
     </row>
@@ -6378,7 +6484,7 @@
         <v>1</v>
       </c>
       <c r="B100" s="6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C100" s="6"/>
       <c r="D100" s="6">
@@ -6386,7 +6492,7 @@
       </c>
       <c r="E100" s="6"/>
       <c r="F100" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G100" s="6"/>
       <c r="H100" s="6">
@@ -6399,7 +6505,7 @@
         <v>2</v>
       </c>
       <c r="B101" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C101" s="6"/>
       <c r="D101" s="6">
@@ -6407,7 +6513,7 @@
       </c>
       <c r="E101" s="6"/>
       <c r="F101" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G101" s="6"/>
       <c r="H101" s="6">
@@ -6420,7 +6526,7 @@
         <v>3</v>
       </c>
       <c r="B102" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C102" s="6"/>
       <c r="D102" s="6">
@@ -6428,7 +6534,7 @@
       </c>
       <c r="E102" s="6"/>
       <c r="F102" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G102" s="6"/>
       <c r="H102" s="6">
@@ -6441,7 +6547,7 @@
         <v>4</v>
       </c>
       <c r="B103" s="6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C103" s="6"/>
       <c r="D103" s="6">
@@ -6449,7 +6555,7 @@
       </c>
       <c r="E103" s="6"/>
       <c r="F103" s="6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G103" s="6"/>
       <c r="H103" s="6">
@@ -6462,7 +6568,7 @@
         <v>5</v>
       </c>
       <c r="B104" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C104" s="9"/>
       <c r="D104" s="9">
@@ -6470,7 +6576,7 @@
       </c>
       <c r="E104" s="9"/>
       <c r="F104" s="9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G104" s="9"/>
       <c r="H104" s="9">
@@ -6481,7 +6587,7 @@
     <row r="107" spans="1:9" ht="14.25" thickBot="1"/>
     <row r="108" spans="1:9">
       <c r="A108" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B108" s="4"/>
       <c r="D108">
@@ -6490,7 +6596,7 @@
     </row>
     <row r="109" spans="1:9">
       <c r="A109" s="5" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B109" s="7">
         <v>3</v>
@@ -6498,7 +6604,7 @@
     </row>
     <row r="110" spans="1:9">
       <c r="A110" s="5" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B110" s="7">
         <v>2</v>
@@ -6506,7 +6612,7 @@
     </row>
     <row r="111" spans="1:9">
       <c r="A111" s="5" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B111" s="7">
         <v>1</v>
@@ -6514,7 +6620,7 @@
     </row>
     <row r="112" spans="1:9">
       <c r="A112" s="5" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B112" s="7">
         <v>2</v>
@@ -6522,7 +6628,7 @@
     </row>
     <row r="113" spans="1:13">
       <c r="A113" s="5" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B113" s="7">
         <v>1</v>
@@ -6530,7 +6636,7 @@
     </row>
     <row r="114" spans="1:13">
       <c r="A114" s="5" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B114" s="7">
         <v>1</v>
@@ -6538,7 +6644,7 @@
     </row>
     <row r="115" spans="1:13">
       <c r="A115" s="5" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B115" s="7">
         <v>1</v>
@@ -6546,21 +6652,21 @@
     </row>
     <row r="116" spans="1:13">
       <c r="A116" s="5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B116" s="7">
         <v>1</v>
       </c>
       <c r="L116" t="s">
+        <v>159</v>
+      </c>
+      <c r="M116" t="s">
         <v>160</v>
-      </c>
-      <c r="M116" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="117" spans="1:13">
       <c r="A117" s="5" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B117" s="7">
         <v>1</v>
@@ -6568,7 +6674,7 @@
     </row>
     <row r="118" spans="1:13">
       <c r="A118" s="5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B118" s="7">
         <v>2</v>
@@ -6576,7 +6682,7 @@
     </row>
     <row r="119" spans="1:13">
       <c r="A119" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B119" s="7">
         <v>3</v>
@@ -6592,7 +6698,7 @@
     </row>
     <row r="121" spans="1:13" ht="14.25" thickBot="1">
       <c r="A121" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B121" s="10">
         <v>1</v>
@@ -6605,7 +6711,7 @@
     </row>
     <row r="127" spans="1:13">
       <c r="B127" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C127" s="3"/>
       <c r="D127" s="3"/>
@@ -6613,13 +6719,13 @@
     </row>
     <row r="128" spans="1:13">
       <c r="B128" s="5" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C128" s="6" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D128" s="6" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E128" s="7"/>
     </row>
@@ -6698,7 +6804,7 @@
       </c>
       <c r="E134" s="7"/>
       <c r="J134" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="K134" s="3"/>
       <c r="L134" s="3"/>
@@ -6716,17 +6822,17 @@
       </c>
       <c r="E135" s="7"/>
       <c r="J135" s="5" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="K135" s="6" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="L135" s="6" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="M135" s="7"/>
       <c r="O135" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="136" spans="2:15">
@@ -6787,7 +6893,7 @@
     </row>
     <row r="139" spans="2:15">
       <c r="B139" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="J139" s="5">
         <v>4</v>
@@ -6873,7 +6979,7 @@
       <c r="E159" s="6"/>
       <c r="F159" s="6"/>
       <c r="O159" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="P159" s="3"/>
       <c r="Q159" s="3"/>
@@ -6881,31 +6987,31 @@
     </row>
     <row r="160" spans="3:18">
       <c r="C160" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D160" s="3"/>
       <c r="E160" s="3"/>
       <c r="F160" s="4"/>
       <c r="O160" s="5" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="P160" s="6" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="Q160" s="6" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="R160" s="7"/>
     </row>
     <row r="161" spans="3:18">
       <c r="C161" s="5" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D161" s="6" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E161" s="6" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F161" s="7"/>
       <c r="O161" s="5">

</xml_diff>